<commit_message>
implementing other metrics cont
</commit_message>
<xml_diff>
--- a/PMConverter/data_analyse/output/C2011-12 Claeys-Verhelst Premises.xlsx
+++ b/PMConverter/data_analyse/output/C2011-12 Claeys-Verhelst Premises.xlsx
@@ -22360,6 +22360,9 @@
       <c r="E2" s="2" t="s">
         <v>317</v>
       </c>
+      <c r="G2" s="6">
+        <v>280520120000</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="6" t="s">
@@ -22789,10 +22792,10 @@
         <v>369</v>
       </c>
       <c r="X3" s="8">
-        <v>-31.5047058703494</v>
+        <v>8427522.29284058</v>
       </c>
       <c r="Y3" s="8">
-        <v>0</v>
+        <v>8381110.80900157</v>
       </c>
       <c r="Z3" s="8">
         <v>-3021447.84066046</v>
@@ -22872,10 +22875,10 @@
         <v>369</v>
       </c>
       <c r="X4" s="8">
-        <v>0</v>
+        <v>8427553.79754645</v>
       </c>
       <c r="Y4" s="8">
-        <v>0</v>
+        <v>8427553.79754645</v>
       </c>
       <c r="Z4" s="8">
         <v>-2773328.61596924</v>
@@ -22955,10 +22958,10 @@
         <v>369</v>
       </c>
       <c r="X5" s="8">
-        <v>-34773.0602731829</v>
+        <v>8392780.73727327</v>
       </c>
       <c r="Y5" s="8">
-        <v>1.16415321826935e-10</v>
+        <v>7974667.03863016</v>
       </c>
       <c r="Z5" s="8">
         <v>-2414830.94463453</v>
@@ -23038,10 +23041,10 @@
         <v>369</v>
       </c>
       <c r="X6" s="8">
-        <v>-67812.876980864</v>
+        <v>8359740.92056559</v>
       </c>
       <c r="Y6" s="8">
-        <v>0</v>
+        <v>7944621.73722862</v>
       </c>
       <c r="Z6" s="8">
         <v>-1911556.68824917</v>
@@ -23121,10 +23124,10 @@
         <v>369</v>
       </c>
       <c r="X7" s="8">
-        <v>-140575.48732702</v>
+        <v>8286978.31021943</v>
       </c>
       <c r="Y7" s="8">
-        <v>0</v>
+        <v>7776296.16459215</v>
       </c>
       <c r="Z7" s="8">
         <v>-1348601.42285757</v>
@@ -23204,10 +23207,10 @@
         <v>369</v>
       </c>
       <c r="X8" s="8">
-        <v>-247992.639614981</v>
+        <v>8179561.15793147</v>
       </c>
       <c r="Y8" s="8">
-        <v>0</v>
+        <v>7660616.2027846</v>
       </c>
       <c r="Z8" s="8">
         <v>-550039.291866797</v>
@@ -23287,10 +23290,10 @@
         <v>373</v>
       </c>
       <c r="X9" s="8">
-        <v>-218880.003967285</v>
+        <v>8208673.79357916</v>
       </c>
       <c r="Y9" s="8">
-        <v>0</v>
+        <v>7859280.38007757</v>
       </c>
       <c r="Z9" s="8">
         <v>0</v>
@@ -23370,10 +23373,10 @@
         <v>373</v>
       </c>
       <c r="X10" s="8">
-        <v>-218880.003967285</v>
+        <v>8208673.79357916</v>
       </c>
       <c r="Y10" s="8">
-        <v>0</v>
+        <v>7859280.38007757</v>
       </c>
       <c r="Z10" s="8">
         <v>0</v>

</xml_diff>

<commit_message>
implemented EAC metrics, todo: implement EAC(t) metrics
</commit_message>
<xml_diff>
--- a/PMConverter/data_analyse/output/C2011-12 Claeys-Verhelst Premises.xlsx
+++ b/PMConverter/data_analyse/output/C2011-12 Claeys-Verhelst Premises.xlsx
@@ -22798,10 +22798,13 @@
         <v>8381110.80900157</v>
       </c>
       <c r="Z3" s="8">
-        <v>-3021447.84066046</v>
+        <v>4459458299.22362</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>0</v>
       </c>
       <c r="AD3" s="8">
-        <v>-1418.00109840903</v>
+        <v>10470053.817495</v>
       </c>
       <c r="AF3" s="10">
         <v>0.00188853603270483</v>
@@ -22881,10 +22884,13 @@
         <v>8427553.79754645</v>
       </c>
       <c r="Z4" s="8">
-        <v>-2773328.61596924</v>
+        <v>97742307.3690326</v>
+      </c>
+      <c r="AA4" s="8">
+        <v>0</v>
       </c>
       <c r="AD4" s="8">
-        <v>-56937.7342795218</v>
+        <v>10261227.4836765</v>
       </c>
       <c r="AF4" s="10">
         <v>0.0838432122023676</v>
@@ -22964,10 +22970,13 @@
         <v>7974667.03863016</v>
       </c>
       <c r="Z5" s="8">
-        <v>-2414830.94463453</v>
+        <v>37010762.5081346</v>
+      </c>
+      <c r="AA5" s="8">
+        <v>0</v>
       </c>
       <c r="AD5" s="8">
-        <v>-116235.011437163</v>
+        <v>9372284.91183462</v>
       </c>
       <c r="AF5" s="10">
         <v>0.213758451287295</v>
@@ -23047,10 +23056,13 @@
         <v>7944621.73722862</v>
       </c>
       <c r="Z6" s="8">
-        <v>-1911556.68824917</v>
+        <v>19646290.8988575</v>
+      </c>
+      <c r="AA6" s="8">
+        <v>0</v>
       </c>
       <c r="AD6" s="8">
-        <v>-161257.569534762</v>
+        <v>8931766.26718367</v>
       </c>
       <c r="AF6" s="10">
         <v>0.39092742276306</v>
@@ -23130,10 +23142,13 @@
         <v>7776296.16459215</v>
       </c>
       <c r="Z7" s="8">
-        <v>-1348601.42285757</v>
+        <v>12675490.7632833</v>
+      </c>
+      <c r="AA7" s="8">
+        <v>0</v>
       </c>
       <c r="AD7" s="8">
-        <v>-164187.983811954</v>
+        <v>8372757.70602897</v>
       </c>
       <c r="AF7" s="10">
         <v>0.600933998841999</v>
@@ -23213,10 +23228,13 @@
         <v>7660616.2027846</v>
       </c>
       <c r="Z8" s="8">
-        <v>-550039.291866797</v>
+        <v>8811618.57160485</v>
+      </c>
+      <c r="AA8" s="8">
+        <v>0</v>
       </c>
       <c r="AD8" s="8">
-        <v>-93413.8110911706</v>
+        <v>7856092.27046979</v>
       </c>
       <c r="AF8" s="10">
         <v>0.900220230268189</v>
@@ -23296,10 +23314,13 @@
         <v>7859280.38007757</v>
       </c>
       <c r="Z9" s="8">
-        <v>0</v>
+        <v>7859280.38007757</v>
+      </c>
+      <c r="AA9" s="8">
+        <v>16834414.9225799</v>
       </c>
       <c r="AD9" s="8">
-        <v>0</v>
+        <v>7859280.38007757</v>
       </c>
       <c r="AF9" s="10">
         <v>1.07230603693811</v>
@@ -23379,10 +23400,13 @@
         <v>7859280.38007757</v>
       </c>
       <c r="Z10" s="8">
-        <v>0</v>
+        <v>7859280.38007757</v>
+      </c>
+      <c r="AA10" s="8">
+        <v>16864894.5732124</v>
       </c>
       <c r="AD10" s="8">
-        <v>0</v>
+        <v>7859280.38007757</v>
       </c>
       <c r="AF10" s="10">
         <v>1.07230603693811</v>

</xml_diff>